<commit_message>
added reset default and fixed sheepwars
</commit_message>
<xml_diff>
--- a/stats.xlsx
+++ b/stats.xlsx
@@ -8578,28 +8578,28 @@
         </is>
       </c>
       <c r="B2" s="4" t="n">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="C2" s="4" t="n">
-        <v>-78</v>
+        <v>-65</v>
       </c>
       <c r="D2" s="4" t="n">
         <v>80</v>
       </c>
       <c r="E2" s="4" t="n">
-        <v>-78</v>
+        <v>-65</v>
       </c>
       <c r="F2" s="4" t="n">
         <v>80</v>
       </c>
       <c r="G2" s="4" t="n">
-        <v>-78</v>
+        <v>-65</v>
       </c>
       <c r="H2" s="4" t="n">
         <v>80</v>
       </c>
       <c r="I2" s="4" t="n">
-        <v>-78</v>
+        <v>-65</v>
       </c>
       <c r="J2" s="4" t="n">
         <v>80</v>
@@ -8612,28 +8612,28 @@
         </is>
       </c>
       <c r="B3" s="6" t="n">
-        <v>2504317.083333332</v>
+        <v>2505057.499999999</v>
       </c>
       <c r="C3" s="4" t="n">
-        <v>16748.75</v>
+        <v>17489.16666666698</v>
       </c>
       <c r="D3" s="6" t="n">
         <v>2487568.333333332</v>
       </c>
       <c r="E3" s="4" t="n">
-        <v>16748.75</v>
+        <v>17489.16666666698</v>
       </c>
       <c r="F3" s="6" t="n">
         <v>2487568.333333332</v>
       </c>
       <c r="G3" s="6" t="n">
-        <v>16748.75000000186</v>
+        <v>17489.16666666884</v>
       </c>
       <c r="H3" s="6" t="n">
         <v>2487568.33333333</v>
       </c>
       <c r="I3" s="4" t="n">
-        <v>16748.75</v>
+        <v>17489.16666666698</v>
       </c>
       <c r="J3" s="6" t="n">
         <v>2487568.333333332</v>
@@ -8646,28 +8646,28 @@
         </is>
       </c>
       <c r="B4" s="4" t="n">
-        <v>513</v>
+        <v>514</v>
       </c>
       <c r="C4" s="4" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D4" s="4" t="n">
         <v>510</v>
       </c>
       <c r="E4" s="4" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F4" s="4" t="n">
         <v>510</v>
       </c>
       <c r="G4" s="4" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H4" s="4" t="n">
         <v>510</v>
       </c>
       <c r="I4" s="4" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J4" s="4" t="n">
         <v>510</v>
@@ -8714,28 +8714,28 @@
         </is>
       </c>
       <c r="B6" s="4" t="n">
-        <v>840059</v>
+        <v>840387</v>
       </c>
       <c r="C6" s="4" t="n">
-        <v>3728</v>
+        <v>4056</v>
       </c>
       <c r="D6" s="4" t="n">
         <v>836331</v>
       </c>
       <c r="E6" s="4" t="n">
-        <v>3728</v>
+        <v>4056</v>
       </c>
       <c r="F6" s="4" t="n">
         <v>836331</v>
       </c>
       <c r="G6" s="4" t="n">
-        <v>3728</v>
+        <v>4056</v>
       </c>
       <c r="H6" s="4" t="n">
         <v>836331</v>
       </c>
       <c r="I6" s="4" t="n">
-        <v>3728</v>
+        <v>4056</v>
       </c>
       <c r="J6" s="4" t="n">
         <v>836331</v>
@@ -8748,28 +8748,28 @@
         </is>
       </c>
       <c r="B7" s="4" t="n">
-        <v>9922</v>
+        <v>9924</v>
       </c>
       <c r="C7" s="4" t="n">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D7" s="4" t="n">
         <v>9910</v>
       </c>
       <c r="E7" s="4" t="n">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="F7" s="4" t="n">
         <v>9910</v>
       </c>
       <c r="G7" s="4" t="n">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="H7" s="4" t="n">
         <v>9910</v>
       </c>
       <c r="I7" s="4" t="n">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="J7" s="4" t="n">
         <v>9910</v>
@@ -8782,28 +8782,28 @@
         </is>
       </c>
       <c r="B8" s="4" t="n">
-        <v>2713</v>
+        <v>2714</v>
       </c>
       <c r="C8" s="4" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D8" s="4" t="n">
         <v>2711</v>
       </c>
       <c r="E8" s="4" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F8" s="4" t="n">
         <v>2711</v>
       </c>
       <c r="G8" s="4" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H8" s="4" t="n">
         <v>2711</v>
       </c>
       <c r="I8" s="4" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J8" s="4" t="n">
         <v>2711</v>
@@ -8816,28 +8816,28 @@
         </is>
       </c>
       <c r="B9" s="4" t="n">
-        <v>24696</v>
+        <v>24705</v>
       </c>
       <c r="C9" s="4" t="n">
-        <v>116</v>
+        <v>125</v>
       </c>
       <c r="D9" s="4" t="n">
         <v>24580</v>
       </c>
       <c r="E9" s="4" t="n">
-        <v>116</v>
+        <v>125</v>
       </c>
       <c r="F9" s="4" t="n">
         <v>24580</v>
       </c>
       <c r="G9" s="4" t="n">
-        <v>116</v>
+        <v>125</v>
       </c>
       <c r="H9" s="4" t="n">
         <v>24580</v>
       </c>
       <c r="I9" s="4" t="n">
-        <v>116</v>
+        <v>125</v>
       </c>
       <c r="J9" s="4" t="n">
         <v>24580</v>
@@ -8850,28 +8850,28 @@
         </is>
       </c>
       <c r="B10" s="4" t="n">
-        <v>6129</v>
+        <v>6131</v>
       </c>
       <c r="C10" s="4" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D10" s="4" t="n">
         <v>6127</v>
       </c>
       <c r="E10" s="4" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F10" s="4" t="n">
         <v>6127</v>
       </c>
       <c r="G10" s="4" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H10" s="4" t="n">
         <v>6127</v>
       </c>
       <c r="I10" s="4" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="J10" s="4" t="n">
         <v>6127</v>
@@ -8884,28 +8884,28 @@
         </is>
       </c>
       <c r="B11" s="4" t="n">
-        <v>308923</v>
+        <v>309039</v>
       </c>
       <c r="C11" s="4" t="n">
-        <v>1255</v>
+        <v>1371</v>
       </c>
       <c r="D11" s="4" t="n">
         <v>307668</v>
       </c>
       <c r="E11" s="4" t="n">
-        <v>1255</v>
+        <v>1371</v>
       </c>
       <c r="F11" s="4" t="n">
         <v>307668</v>
       </c>
       <c r="G11" s="4" t="n">
-        <v>1255</v>
+        <v>1371</v>
       </c>
       <c r="H11" s="4" t="n">
         <v>307668</v>
       </c>
       <c r="I11" s="4" t="n">
-        <v>1255</v>
+        <v>1371</v>
       </c>
       <c r="J11" s="4" t="n">
         <v>307668</v>
@@ -8952,28 +8952,28 @@
         </is>
       </c>
       <c r="B13" s="4" t="n">
-        <v>6817</v>
+        <v>6818</v>
       </c>
       <c r="C13" s="4" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D13" s="4" t="n">
         <v>6807</v>
       </c>
       <c r="E13" s="4" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F13" s="4" t="n">
         <v>6807</v>
       </c>
       <c r="G13" s="4" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H13" s="4" t="n">
         <v>6807</v>
       </c>
       <c r="I13" s="4" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="J13" s="4" t="n">
         <v>6807</v>
@@ -8986,28 +8986,28 @@
         </is>
       </c>
       <c r="B14" s="4" t="n">
-        <v>18549</v>
+        <v>18556</v>
       </c>
       <c r="C14" s="4" t="n">
-        <v>114</v>
+        <v>121</v>
       </c>
       <c r="D14" s="4" t="n">
         <v>18435</v>
       </c>
       <c r="E14" s="4" t="n">
-        <v>114</v>
+        <v>121</v>
       </c>
       <c r="F14" s="4" t="n">
         <v>18435</v>
       </c>
       <c r="G14" s="4" t="n">
-        <v>114</v>
+        <v>121</v>
       </c>
       <c r="H14" s="4" t="n">
         <v>18435</v>
       </c>
       <c r="I14" s="4" t="n">
-        <v>114</v>
+        <v>121</v>
       </c>
       <c r="J14" s="4" t="n">
         <v>18435</v>
@@ -9020,28 +9020,28 @@
         </is>
       </c>
       <c r="B15" s="4" t="n">
-        <v>36038</v>
+        <v>36053</v>
       </c>
       <c r="C15" s="4" t="n">
-        <v>196</v>
+        <v>211</v>
       </c>
       <c r="D15" s="4" t="n">
         <v>35842</v>
       </c>
       <c r="E15" s="4" t="n">
-        <v>196</v>
+        <v>211</v>
       </c>
       <c r="F15" s="4" t="n">
         <v>35842</v>
       </c>
       <c r="G15" s="4" t="n">
-        <v>196</v>
+        <v>211</v>
       </c>
       <c r="H15" s="4" t="n">
         <v>35842</v>
       </c>
       <c r="I15" s="4" t="n">
-        <v>196</v>
+        <v>211</v>
       </c>
       <c r="J15" s="4" t="n">
         <v>35842</v>
@@ -9054,28 +9054,28 @@
         </is>
       </c>
       <c r="B16" s="4" t="n">
-        <v>22937</v>
+        <v>22943</v>
       </c>
       <c r="C16" s="4" t="n">
-        <v>122</v>
+        <v>128</v>
       </c>
       <c r="D16" s="4" t="n">
         <v>22815</v>
       </c>
       <c r="E16" s="4" t="n">
-        <v>122</v>
+        <v>128</v>
       </c>
       <c r="F16" s="4" t="n">
         <v>22815</v>
       </c>
       <c r="G16" s="4" t="n">
-        <v>122</v>
+        <v>128</v>
       </c>
       <c r="H16" s="4" t="n">
         <v>22815</v>
       </c>
       <c r="I16" s="4" t="n">
-        <v>122</v>
+        <v>128</v>
       </c>
       <c r="J16" s="4" t="n">
         <v>22815</v>
@@ -9088,28 +9088,28 @@
         </is>
       </c>
       <c r="B17" s="4" t="n">
-        <v>17801</v>
+        <v>17809</v>
       </c>
       <c r="C17" s="4" t="n">
-        <v>90</v>
+        <v>98</v>
       </c>
       <c r="D17" s="4" t="n">
         <v>17711</v>
       </c>
       <c r="E17" s="4" t="n">
-        <v>90</v>
+        <v>98</v>
       </c>
       <c r="F17" s="4" t="n">
         <v>17711</v>
       </c>
       <c r="G17" s="4" t="n">
-        <v>90</v>
+        <v>98</v>
       </c>
       <c r="H17" s="4" t="n">
         <v>17711</v>
       </c>
       <c r="I17" s="4" t="n">
-        <v>90</v>
+        <v>98</v>
       </c>
       <c r="J17" s="4" t="n">
         <v>17711</v>
@@ -9122,28 +9122,28 @@
         </is>
       </c>
       <c r="B18" s="4" t="n">
-        <v>11577</v>
+        <v>11585</v>
       </c>
       <c r="C18" s="4" t="n">
-        <v>63</v>
+        <v>71</v>
       </c>
       <c r="D18" s="4" t="n">
         <v>11514</v>
       </c>
       <c r="E18" s="4" t="n">
-        <v>63</v>
+        <v>71</v>
       </c>
       <c r="F18" s="4" t="n">
         <v>11514</v>
       </c>
       <c r="G18" s="4" t="n">
-        <v>63</v>
+        <v>71</v>
       </c>
       <c r="H18" s="4" t="n">
         <v>11514</v>
       </c>
       <c r="I18" s="4" t="n">
-        <v>63</v>
+        <v>71</v>
       </c>
       <c r="J18" s="4" t="n">
         <v>11514</v>
@@ -9224,28 +9224,28 @@
         </is>
       </c>
       <c r="B21" s="4" t="n">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="C21" s="4" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D21" s="4" t="n">
         <v>1199</v>
       </c>
       <c r="E21" s="4" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F21" s="4" t="n">
         <v>1199</v>
       </c>
       <c r="G21" s="4" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="H21" s="4" t="n">
         <v>1199</v>
       </c>
       <c r="I21" s="4" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="J21" s="4" t="n">
         <v>1199</v>
@@ -9258,28 +9258,28 @@
         </is>
       </c>
       <c r="B22" s="4" t="n">
-        <v>2845227</v>
+        <v>2846128</v>
       </c>
       <c r="C22" s="4" t="n">
-        <v>13269</v>
+        <v>14170</v>
       </c>
       <c r="D22" s="4" t="n">
         <v>2831958</v>
       </c>
       <c r="E22" s="4" t="n">
-        <v>13269</v>
+        <v>14170</v>
       </c>
       <c r="F22" s="4" t="n">
         <v>2831958</v>
       </c>
       <c r="G22" s="4" t="n">
-        <v>13269</v>
+        <v>14170</v>
       </c>
       <c r="H22" s="4" t="n">
         <v>2831958</v>
       </c>
       <c r="I22" s="4" t="n">
-        <v>13269</v>
+        <v>14170</v>
       </c>
       <c r="J22" s="4" t="n">
         <v>2831958</v>
@@ -24028,28 +24028,28 @@
         </is>
       </c>
       <c r="B2" t="n">
+        <v>65</v>
+      </c>
+      <c r="C2" t="n">
         <v>60</v>
-      </c>
-      <c r="C2" t="n">
-        <v>55</v>
       </c>
       <c r="D2" t="n">
         <v>5</v>
       </c>
       <c r="E2" t="n">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="F2" t="n">
         <v>5</v>
       </c>
       <c r="G2" t="n">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="H2" t="n">
         <v>5</v>
       </c>
       <c r="I2" t="n">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="J2" t="n">
         <v>5</v>
@@ -24062,28 +24062,28 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>188492.9166666667</v>
+        <v>189387.9166666667</v>
       </c>
       <c r="C3" t="n">
-        <v>36217.50000000015</v>
+        <v>37112.50000000017</v>
       </c>
       <c r="D3" t="n">
         <v>152275.4166666665</v>
       </c>
       <c r="E3" t="n">
-        <v>36217.50000000015</v>
+        <v>37112.50000000017</v>
       </c>
       <c r="F3" t="n">
         <v>152275.4166666665</v>
       </c>
       <c r="G3" t="n">
-        <v>36217.50000000015</v>
+        <v>37112.50000000017</v>
       </c>
       <c r="H3" t="n">
         <v>152275.4166666665</v>
       </c>
       <c r="I3" t="n">
-        <v>36217.50000000015</v>
+        <v>37112.50000000017</v>
       </c>
       <c r="J3" t="n">
         <v>152275.4166666665</v>
@@ -24164,28 +24164,28 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>39377</v>
+        <v>39546</v>
       </c>
       <c r="C6" t="n">
-        <v>8017</v>
+        <v>8186</v>
       </c>
       <c r="D6" t="n">
         <v>31360</v>
       </c>
       <c r="E6" t="n">
-        <v>8017</v>
+        <v>8186</v>
       </c>
       <c r="F6" t="n">
         <v>31360</v>
       </c>
       <c r="G6" t="n">
-        <v>8017</v>
+        <v>8186</v>
       </c>
       <c r="H6" t="n">
         <v>31360</v>
       </c>
       <c r="I6" t="n">
-        <v>8017</v>
+        <v>8186</v>
       </c>
       <c r="J6" t="n">
         <v>31360</v>
@@ -24198,28 +24198,28 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>1104</v>
+        <v>1108</v>
       </c>
       <c r="C7" t="n">
-        <v>154</v>
+        <v>158</v>
       </c>
       <c r="D7" t="n">
         <v>950</v>
       </c>
       <c r="E7" t="n">
-        <v>154</v>
+        <v>158</v>
       </c>
       <c r="F7" t="n">
         <v>950</v>
       </c>
       <c r="G7" t="n">
-        <v>154</v>
+        <v>158</v>
       </c>
       <c r="H7" t="n">
         <v>950</v>
       </c>
       <c r="I7" t="n">
-        <v>154</v>
+        <v>158</v>
       </c>
       <c r="J7" t="n">
         <v>950</v>
@@ -24232,28 +24232,28 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="C8" t="n">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D8" t="n">
         <v>151</v>
       </c>
       <c r="E8" t="n">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="F8" t="n">
         <v>151</v>
       </c>
       <c r="G8" t="n">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="H8" t="n">
         <v>151</v>
       </c>
       <c r="I8" t="n">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="J8" t="n">
         <v>151</v>
@@ -24266,28 +24266,28 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>2113</v>
+        <v>2126</v>
       </c>
       <c r="C9" t="n">
-        <v>447</v>
+        <v>460</v>
       </c>
       <c r="D9" t="n">
         <v>1666</v>
       </c>
       <c r="E9" t="n">
-        <v>447</v>
+        <v>460</v>
       </c>
       <c r="F9" t="n">
         <v>1666</v>
       </c>
       <c r="G9" t="n">
-        <v>447</v>
+        <v>460</v>
       </c>
       <c r="H9" t="n">
         <v>1666</v>
       </c>
       <c r="I9" t="n">
-        <v>447</v>
+        <v>460</v>
       </c>
       <c r="J9" t="n">
         <v>1666</v>
@@ -24300,28 +24300,28 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>786</v>
+        <v>789</v>
       </c>
       <c r="C10" t="n">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="D10" t="n">
         <v>692</v>
       </c>
       <c r="E10" t="n">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="F10" t="n">
         <v>692</v>
       </c>
       <c r="G10" t="n">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="H10" t="n">
         <v>692</v>
       </c>
       <c r="I10" t="n">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="J10" t="n">
         <v>692</v>
@@ -24334,28 +24334,28 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>26991</v>
+        <v>27112</v>
       </c>
       <c r="C11" t="n">
-        <v>4889</v>
+        <v>5010</v>
       </c>
       <c r="D11" t="n">
         <v>22102</v>
       </c>
       <c r="E11" t="n">
-        <v>4889</v>
+        <v>5010</v>
       </c>
       <c r="F11" t="n">
         <v>22102</v>
       </c>
       <c r="G11" t="n">
-        <v>4889</v>
+        <v>5010</v>
       </c>
       <c r="H11" t="n">
         <v>22102</v>
       </c>
       <c r="I11" t="n">
-        <v>4889</v>
+        <v>5010</v>
       </c>
       <c r="J11" t="n">
         <v>22102</v>
@@ -24402,28 +24402,28 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>773</v>
+        <v>775</v>
       </c>
       <c r="C13" t="n">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="D13" t="n">
         <v>651</v>
       </c>
       <c r="E13" t="n">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="F13" t="n">
         <v>651</v>
       </c>
       <c r="G13" t="n">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="H13" t="n">
         <v>651</v>
       </c>
       <c r="I13" t="n">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="J13" t="n">
         <v>651</v>
@@ -24436,28 +24436,28 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>1327</v>
+        <v>1337</v>
       </c>
       <c r="C14" t="n">
-        <v>353</v>
+        <v>363</v>
       </c>
       <c r="D14" t="n">
         <v>974</v>
       </c>
       <c r="E14" t="n">
-        <v>353</v>
+        <v>363</v>
       </c>
       <c r="F14" t="n">
         <v>974</v>
       </c>
       <c r="G14" t="n">
-        <v>353</v>
+        <v>363</v>
       </c>
       <c r="H14" t="n">
         <v>974</v>
       </c>
       <c r="I14" t="n">
-        <v>353</v>
+        <v>363</v>
       </c>
       <c r="J14" t="n">
         <v>974</v>
@@ -24470,28 +24470,28 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>1827</v>
+        <v>1834</v>
       </c>
       <c r="C15" t="n">
-        <v>319</v>
+        <v>326</v>
       </c>
       <c r="D15" t="n">
         <v>1508</v>
       </c>
       <c r="E15" t="n">
-        <v>319</v>
+        <v>326</v>
       </c>
       <c r="F15" t="n">
         <v>1508</v>
       </c>
       <c r="G15" t="n">
-        <v>319</v>
+        <v>326</v>
       </c>
       <c r="H15" t="n">
         <v>1508</v>
       </c>
       <c r="I15" t="n">
-        <v>319</v>
+        <v>326</v>
       </c>
       <c r="J15" t="n">
         <v>1508</v>
@@ -24504,28 +24504,28 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>1163</v>
+        <v>1167</v>
       </c>
       <c r="C16" t="n">
-        <v>206</v>
+        <v>210</v>
       </c>
       <c r="D16" t="n">
         <v>957</v>
       </c>
       <c r="E16" t="n">
-        <v>206</v>
+        <v>210</v>
       </c>
       <c r="F16" t="n">
         <v>957</v>
       </c>
       <c r="G16" t="n">
-        <v>206</v>
+        <v>210</v>
       </c>
       <c r="H16" t="n">
         <v>957</v>
       </c>
       <c r="I16" t="n">
-        <v>206</v>
+        <v>210</v>
       </c>
       <c r="J16" t="n">
         <v>957</v>
@@ -24538,28 +24538,28 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>595</v>
+        <v>599</v>
       </c>
       <c r="C17" t="n">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="D17" t="n">
         <v>451</v>
       </c>
       <c r="E17" t="n">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="F17" t="n">
         <v>451</v>
       </c>
       <c r="G17" t="n">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="H17" t="n">
         <v>451</v>
       </c>
       <c r="I17" t="n">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="J17" t="n">
         <v>451</v>
@@ -24572,28 +24572,28 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>455</v>
+        <v>458</v>
       </c>
       <c r="C18" t="n">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="D18" t="n">
         <v>348</v>
       </c>
       <c r="E18" t="n">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="F18" t="n">
         <v>348</v>
       </c>
       <c r="G18" t="n">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="H18" t="n">
         <v>348</v>
       </c>
       <c r="I18" t="n">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="J18" t="n">
         <v>348</v>
@@ -24708,28 +24708,28 @@
         </is>
       </c>
       <c r="B22" t="n">
-        <v>222519</v>
+        <v>223827</v>
       </c>
       <c r="C22" t="n">
-        <v>47238</v>
+        <v>48546</v>
       </c>
       <c r="D22" t="n">
         <v>175281</v>
       </c>
       <c r="E22" t="n">
-        <v>47238</v>
+        <v>48546</v>
       </c>
       <c r="F22" t="n">
         <v>175281</v>
       </c>
       <c r="G22" t="n">
-        <v>47238</v>
+        <v>48546</v>
       </c>
       <c r="H22" t="n">
         <v>175281</v>
       </c>
       <c r="I22" t="n">
-        <v>47238</v>
+        <v>48546</v>
       </c>
       <c r="J22" t="n">
         <v>175281</v>
@@ -24813,28 +24813,28 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>89</v>
+        <v>4</v>
       </c>
       <c r="C2" t="n">
-        <v>89</v>
+        <v>4</v>
       </c>
       <c r="D2" t="n">
         <v>0</v>
       </c>
       <c r="E2" t="n">
-        <v>89</v>
+        <v>4</v>
       </c>
       <c r="F2" t="n">
         <v>0</v>
       </c>
       <c r="G2" t="n">
-        <v>89</v>
+        <v>4</v>
       </c>
       <c r="H2" t="n">
         <v>0</v>
       </c>
       <c r="I2" t="n">
-        <v>89</v>
+        <v>4</v>
       </c>
       <c r="J2" t="n">
         <v>0</v>
@@ -24847,28 +24847,28 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>196073.7499999997</v>
+        <v>213425.8333333331</v>
       </c>
       <c r="C3" t="n">
-        <v>14382.9166666666</v>
+        <v>31735</v>
       </c>
       <c r="D3" t="n">
         <v>181690.8333333331</v>
       </c>
       <c r="E3" t="n">
-        <v>14382.9166666666</v>
+        <v>31735</v>
       </c>
       <c r="F3" t="n">
         <v>181690.8333333331</v>
       </c>
       <c r="G3" t="n">
-        <v>14382.9166666666</v>
+        <v>31735</v>
       </c>
       <c r="H3" t="n">
         <v>181690.8333333331</v>
       </c>
       <c r="I3" t="n">
-        <v>14382.9166666666</v>
+        <v>31735</v>
       </c>
       <c r="J3" t="n">
         <v>181690.8333333331</v>
@@ -24881,28 +24881,28 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="C4" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D4" t="n">
         <v>39</v>
       </c>
       <c r="E4" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="F4" t="n">
         <v>39</v>
       </c>
       <c r="G4" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="H4" t="n">
         <v>39</v>
       </c>
       <c r="I4" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="J4" t="n">
         <v>39</v>
@@ -24915,28 +24915,28 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>57070</v>
+        <v>59760</v>
       </c>
       <c r="C5" t="n">
-        <v>830</v>
+        <v>3520</v>
       </c>
       <c r="D5" t="n">
         <v>56240</v>
       </c>
       <c r="E5" t="n">
-        <v>830</v>
+        <v>3520</v>
       </c>
       <c r="F5" t="n">
         <v>56240</v>
       </c>
       <c r="G5" t="n">
-        <v>830</v>
+        <v>3520</v>
       </c>
       <c r="H5" t="n">
         <v>56240</v>
       </c>
       <c r="I5" t="n">
-        <v>830</v>
+        <v>3520</v>
       </c>
       <c r="J5" t="n">
         <v>56240</v>
@@ -24949,28 +24949,28 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>70296</v>
+        <v>75006</v>
       </c>
       <c r="C6" t="n">
-        <v>4667</v>
+        <v>9377</v>
       </c>
       <c r="D6" t="n">
         <v>65629</v>
       </c>
       <c r="E6" t="n">
-        <v>4667</v>
+        <v>9377</v>
       </c>
       <c r="F6" t="n">
         <v>65629</v>
       </c>
       <c r="G6" t="n">
-        <v>4667</v>
+        <v>9377</v>
       </c>
       <c r="H6" t="n">
         <v>65629</v>
       </c>
       <c r="I6" t="n">
-        <v>4667</v>
+        <v>9377</v>
       </c>
       <c r="J6" t="n">
         <v>65629</v>
@@ -24983,28 +24983,28 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>1069</v>
+        <v>1116</v>
       </c>
       <c r="C7" t="n">
-        <v>60</v>
+        <v>107</v>
       </c>
       <c r="D7" t="n">
         <v>1009</v>
       </c>
       <c r="E7" t="n">
-        <v>60</v>
+        <v>107</v>
       </c>
       <c r="F7" t="n">
         <v>1009</v>
       </c>
       <c r="G7" t="n">
-        <v>60</v>
+        <v>107</v>
       </c>
       <c r="H7" t="n">
         <v>1009</v>
       </c>
       <c r="I7" t="n">
-        <v>60</v>
+        <v>107</v>
       </c>
       <c r="J7" t="n">
         <v>1009</v>
@@ -25017,28 +25017,28 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>135</v>
+        <v>142</v>
       </c>
       <c r="C8" t="n">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="D8" t="n">
         <v>121</v>
       </c>
       <c r="E8" t="n">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="F8" t="n">
         <v>121</v>
       </c>
       <c r="G8" t="n">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="H8" t="n">
         <v>121</v>
       </c>
       <c r="I8" t="n">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="J8" t="n">
         <v>121</v>
@@ -25051,28 +25051,28 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>2256</v>
+        <v>2418</v>
       </c>
       <c r="C9" t="n">
-        <v>161</v>
+        <v>323</v>
       </c>
       <c r="D9" t="n">
         <v>2095</v>
       </c>
       <c r="E9" t="n">
-        <v>161</v>
+        <v>323</v>
       </c>
       <c r="F9" t="n">
         <v>2095</v>
       </c>
       <c r="G9" t="n">
-        <v>161</v>
+        <v>323</v>
       </c>
       <c r="H9" t="n">
         <v>2095</v>
       </c>
       <c r="I9" t="n">
-        <v>161</v>
+        <v>323</v>
       </c>
       <c r="J9" t="n">
         <v>2095</v>
@@ -25085,28 +25085,28 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>615</v>
+        <v>648</v>
       </c>
       <c r="C10" t="n">
-        <v>31</v>
+        <v>64</v>
       </c>
       <c r="D10" t="n">
         <v>584</v>
       </c>
       <c r="E10" t="n">
-        <v>31</v>
+        <v>64</v>
       </c>
       <c r="F10" t="n">
         <v>584</v>
       </c>
       <c r="G10" t="n">
-        <v>31</v>
+        <v>64</v>
       </c>
       <c r="H10" t="n">
         <v>584</v>
       </c>
       <c r="I10" t="n">
-        <v>31</v>
+        <v>64</v>
       </c>
       <c r="J10" t="n">
         <v>584</v>
@@ -25119,28 +25119,28 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>28681</v>
+        <v>30195</v>
       </c>
       <c r="C11" t="n">
-        <v>1474</v>
+        <v>2988</v>
       </c>
       <c r="D11" t="n">
         <v>27207</v>
       </c>
       <c r="E11" t="n">
-        <v>1474</v>
+        <v>2988</v>
       </c>
       <c r="F11" t="n">
         <v>27207</v>
       </c>
       <c r="G11" t="n">
-        <v>1474</v>
+        <v>2988</v>
       </c>
       <c r="H11" t="n">
         <v>27207</v>
       </c>
       <c r="I11" t="n">
-        <v>1474</v>
+        <v>2988</v>
       </c>
       <c r="J11" t="n">
         <v>27207</v>
@@ -25153,28 +25153,28 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C12" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D12" t="n">
         <v>5</v>
       </c>
       <c r="E12" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F12" t="n">
         <v>5</v>
       </c>
       <c r="G12" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H12" t="n">
         <v>5</v>
       </c>
       <c r="I12" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J12" t="n">
         <v>5</v>
@@ -25187,28 +25187,28 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>367</v>
+        <v>405</v>
       </c>
       <c r="C13" t="n">
-        <v>44</v>
+        <v>82</v>
       </c>
       <c r="D13" t="n">
         <v>323</v>
       </c>
       <c r="E13" t="n">
-        <v>44</v>
+        <v>82</v>
       </c>
       <c r="F13" t="n">
         <v>323</v>
       </c>
       <c r="G13" t="n">
-        <v>44</v>
+        <v>82</v>
       </c>
       <c r="H13" t="n">
         <v>323</v>
       </c>
       <c r="I13" t="n">
-        <v>44</v>
+        <v>82</v>
       </c>
       <c r="J13" t="n">
         <v>323</v>
@@ -25221,28 +25221,28 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>1641</v>
+        <v>1770</v>
       </c>
       <c r="C14" t="n">
-        <v>130</v>
+        <v>259</v>
       </c>
       <c r="D14" t="n">
         <v>1511</v>
       </c>
       <c r="E14" t="n">
-        <v>130</v>
+        <v>259</v>
       </c>
       <c r="F14" t="n">
         <v>1511</v>
       </c>
       <c r="G14" t="n">
-        <v>130</v>
+        <v>259</v>
       </c>
       <c r="H14" t="n">
         <v>1511</v>
       </c>
       <c r="I14" t="n">
-        <v>130</v>
+        <v>259</v>
       </c>
       <c r="J14" t="n">
         <v>1511</v>
@@ -25255,28 +25255,28 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>3715</v>
+        <v>3918</v>
       </c>
       <c r="C15" t="n">
-        <v>215</v>
+        <v>418</v>
       </c>
       <c r="D15" t="n">
         <v>3500</v>
       </c>
       <c r="E15" t="n">
-        <v>215</v>
+        <v>418</v>
       </c>
       <c r="F15" t="n">
         <v>3500</v>
       </c>
       <c r="G15" t="n">
-        <v>215</v>
+        <v>418</v>
       </c>
       <c r="H15" t="n">
         <v>3500</v>
       </c>
       <c r="I15" t="n">
-        <v>215</v>
+        <v>418</v>
       </c>
       <c r="J15" t="n">
         <v>3500</v>
@@ -25289,28 +25289,28 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>1076</v>
+        <v>1204</v>
       </c>
       <c r="C16" t="n">
-        <v>118</v>
+        <v>246</v>
       </c>
       <c r="D16" t="n">
         <v>958</v>
       </c>
       <c r="E16" t="n">
-        <v>118</v>
+        <v>246</v>
       </c>
       <c r="F16" t="n">
         <v>958</v>
       </c>
       <c r="G16" t="n">
-        <v>118</v>
+        <v>246</v>
       </c>
       <c r="H16" t="n">
         <v>958</v>
       </c>
       <c r="I16" t="n">
-        <v>118</v>
+        <v>246</v>
       </c>
       <c r="J16" t="n">
         <v>958</v>
@@ -25323,28 +25323,28 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>692</v>
+        <v>765</v>
       </c>
       <c r="C17" t="n">
-        <v>55</v>
+        <v>128</v>
       </c>
       <c r="D17" t="n">
         <v>637</v>
       </c>
       <c r="E17" t="n">
-        <v>55</v>
+        <v>128</v>
       </c>
       <c r="F17" t="n">
         <v>637</v>
       </c>
       <c r="G17" t="n">
-        <v>55</v>
+        <v>128</v>
       </c>
       <c r="H17" t="n">
         <v>637</v>
       </c>
       <c r="I17" t="n">
-        <v>55</v>
+        <v>128</v>
       </c>
       <c r="J17" t="n">
         <v>637</v>
@@ -25357,28 +25357,28 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>482</v>
+        <v>541</v>
       </c>
       <c r="C18" t="n">
-        <v>72</v>
+        <v>131</v>
       </c>
       <c r="D18" t="n">
         <v>410</v>
       </c>
       <c r="E18" t="n">
-        <v>72</v>
+        <v>131</v>
       </c>
       <c r="F18" t="n">
         <v>410</v>
       </c>
       <c r="G18" t="n">
-        <v>72</v>
+        <v>131</v>
       </c>
       <c r="H18" t="n">
         <v>410</v>
       </c>
       <c r="I18" t="n">
-        <v>72</v>
+        <v>131</v>
       </c>
       <c r="J18" t="n">
         <v>410</v>
@@ -25391,28 +25391,28 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>93</v>
+        <v>102</v>
       </c>
       <c r="C19" t="n">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="D19" t="n">
         <v>83</v>
       </c>
       <c r="E19" t="n">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="F19" t="n">
         <v>83</v>
       </c>
       <c r="G19" t="n">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="H19" t="n">
         <v>83</v>
       </c>
       <c r="I19" t="n">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="J19" t="n">
         <v>83</v>
@@ -25459,28 +25459,28 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>91</v>
+        <v>98</v>
       </c>
       <c r="C21" t="n">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="D21" t="n">
         <v>76</v>
       </c>
       <c r="E21" t="n">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="F21" t="n">
         <v>76</v>
       </c>
       <c r="G21" t="n">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="H21" t="n">
         <v>76</v>
       </c>
       <c r="I21" t="n">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="J21" t="n">
         <v>76</v>
@@ -25493,28 +25493,28 @@
         </is>
       </c>
       <c r="B22" t="n">
-        <v>140571</v>
+        <v>158828</v>
       </c>
       <c r="C22" t="n">
-        <v>17803</v>
+        <v>36060</v>
       </c>
       <c r="D22" t="n">
         <v>122768</v>
       </c>
       <c r="E22" t="n">
-        <v>17803</v>
+        <v>36060</v>
       </c>
       <c r="F22" t="n">
         <v>122768</v>
       </c>
       <c r="G22" t="n">
-        <v>17803</v>
+        <v>36060</v>
       </c>
       <c r="H22" t="n">
         <v>122768</v>
       </c>
       <c r="I22" t="n">
-        <v>17803</v>
+        <v>36060</v>
       </c>
       <c r="J22" t="n">
         <v>122768</v>
@@ -25610,28 +25610,28 @@
         </is>
       </c>
       <c r="B2" s="4" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C2" s="4" t="n">
-        <v>-48</v>
+        <v>-50</v>
       </c>
       <c r="D2" s="4" t="n">
         <v>51</v>
       </c>
       <c r="E2" s="4" t="n">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="F2" s="4" t="n">
         <v>3</v>
       </c>
       <c r="G2" s="4" t="n">
-        <v>-7</v>
+        <v>-9</v>
       </c>
       <c r="H2" s="4" t="n">
         <v>10</v>
       </c>
       <c r="I2" s="4" t="n">
-        <v>-48</v>
+        <v>-50</v>
       </c>
       <c r="J2" s="4" t="n">
         <v>51</v>
@@ -25712,28 +25712,28 @@
         </is>
       </c>
       <c r="B5" s="4" t="n">
-        <v>142523</v>
+        <v>142545</v>
       </c>
       <c r="C5" s="4" t="n">
-        <v>1211</v>
+        <v>1233</v>
       </c>
       <c r="D5" s="4" t="n">
         <v>141312</v>
       </c>
       <c r="E5" s="4" t="n">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="F5" s="4" t="n">
         <v>142523</v>
       </c>
       <c r="G5" s="4" t="n">
-        <v>3523</v>
+        <v>3545</v>
       </c>
       <c r="H5" s="4" t="n">
         <v>139000</v>
       </c>
       <c r="I5" s="4" t="n">
-        <v>1211</v>
+        <v>1233</v>
       </c>
       <c r="J5" s="4" t="n">
         <v>141312</v>
@@ -27214,28 +27214,28 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>1673229.999999998</v>
+        <v>1673969.583333331</v>
       </c>
       <c r="C3" t="n">
-        <v>32714.16666666511</v>
+        <v>33453.74999999814</v>
       </c>
       <c r="D3" t="n">
         <v>1640515.833333333</v>
       </c>
       <c r="E3" t="n">
-        <v>32714.16666666511</v>
+        <v>33453.74999999814</v>
       </c>
       <c r="F3" t="n">
         <v>1640515.833333333</v>
       </c>
       <c r="G3" t="n">
-        <v>32714.16666666511</v>
+        <v>33453.74999999814</v>
       </c>
       <c r="H3" t="n">
         <v>1640515.833333333</v>
       </c>
       <c r="I3" t="n">
-        <v>32714.16666666511</v>
+        <v>33453.74999999814</v>
       </c>
       <c r="J3" t="n">
         <v>1640515.833333333</v>
@@ -27282,28 +27282,28 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>174807</v>
+        <v>174837</v>
       </c>
       <c r="C5" t="n">
-        <v>911</v>
+        <v>941</v>
       </c>
       <c r="D5" t="n">
         <v>173896</v>
       </c>
       <c r="E5" t="n">
-        <v>911</v>
+        <v>941</v>
       </c>
       <c r="F5" t="n">
         <v>173896</v>
       </c>
       <c r="G5" t="n">
-        <v>911</v>
+        <v>941</v>
       </c>
       <c r="H5" t="n">
         <v>173896</v>
       </c>
       <c r="I5" t="n">
-        <v>911</v>
+        <v>941</v>
       </c>
       <c r="J5" t="n">
         <v>173896</v>
@@ -27316,28 +27316,28 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>627091</v>
+        <v>627196</v>
       </c>
       <c r="C6" t="n">
-        <v>13376</v>
+        <v>13481</v>
       </c>
       <c r="D6" t="n">
         <v>613715</v>
       </c>
       <c r="E6" t="n">
-        <v>13376</v>
+        <v>13481</v>
       </c>
       <c r="F6" t="n">
         <v>613715</v>
       </c>
       <c r="G6" t="n">
-        <v>13376</v>
+        <v>13481</v>
       </c>
       <c r="H6" t="n">
         <v>613715</v>
       </c>
       <c r="I6" t="n">
-        <v>13376</v>
+        <v>13481</v>
       </c>
       <c r="J6" t="n">
         <v>613715</v>
@@ -27350,28 +27350,28 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>8951</v>
+        <v>8953</v>
       </c>
       <c r="C7" t="n">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="D7" t="n">
         <v>8863</v>
       </c>
       <c r="E7" t="n">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="F7" t="n">
         <v>8863</v>
       </c>
       <c r="G7" t="n">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="H7" t="n">
         <v>8863</v>
       </c>
       <c r="I7" t="n">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="J7" t="n">
         <v>8863</v>
@@ -27384,28 +27384,28 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>2231</v>
+        <v>2232</v>
       </c>
       <c r="C8" t="n">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D8" t="n">
         <v>2212</v>
       </c>
       <c r="E8" t="n">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F8" t="n">
         <v>2212</v>
       </c>
       <c r="G8" t="n">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H8" t="n">
         <v>2212</v>
       </c>
       <c r="I8" t="n">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="J8" t="n">
         <v>2212</v>
@@ -27418,28 +27418,28 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>19508</v>
+        <v>19514</v>
       </c>
       <c r="C9" t="n">
-        <v>409</v>
+        <v>415</v>
       </c>
       <c r="D9" t="n">
         <v>19099</v>
       </c>
       <c r="E9" t="n">
-        <v>409</v>
+        <v>415</v>
       </c>
       <c r="F9" t="n">
         <v>19099</v>
       </c>
       <c r="G9" t="n">
-        <v>409</v>
+        <v>415</v>
       </c>
       <c r="H9" t="n">
         <v>19099</v>
       </c>
       <c r="I9" t="n">
-        <v>409</v>
+        <v>415</v>
       </c>
       <c r="J9" t="n">
         <v>19099</v>
@@ -27452,28 +27452,28 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>6225</v>
+        <v>6227</v>
       </c>
       <c r="C10" t="n">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="D10" t="n">
         <v>6172</v>
       </c>
       <c r="E10" t="n">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="F10" t="n">
         <v>6172</v>
       </c>
       <c r="G10" t="n">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="H10" t="n">
         <v>6172</v>
       </c>
       <c r="I10" t="n">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="J10" t="n">
         <v>6172</v>
@@ -27486,28 +27486,28 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>241356</v>
+        <v>241406</v>
       </c>
       <c r="C11" t="n">
-        <v>4726</v>
+        <v>4776</v>
       </c>
       <c r="D11" t="n">
         <v>236630</v>
       </c>
       <c r="E11" t="n">
-        <v>4726</v>
+        <v>4776</v>
       </c>
       <c r="F11" t="n">
         <v>236630</v>
       </c>
       <c r="G11" t="n">
-        <v>4726</v>
+        <v>4776</v>
       </c>
       <c r="H11" t="n">
         <v>236630</v>
       </c>
       <c r="I11" t="n">
-        <v>4726</v>
+        <v>4776</v>
       </c>
       <c r="J11" t="n">
         <v>236630</v>
@@ -27554,28 +27554,28 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>6379</v>
+        <v>6380</v>
       </c>
       <c r="C13" t="n">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D13" t="n">
         <v>6312</v>
       </c>
       <c r="E13" t="n">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="F13" t="n">
         <v>6312</v>
       </c>
       <c r="G13" t="n">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="H13" t="n">
         <v>6312</v>
       </c>
       <c r="I13" t="n">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="J13" t="n">
         <v>6312</v>
@@ -27588,28 +27588,28 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>13258</v>
+        <v>13262</v>
       </c>
       <c r="C14" t="n">
-        <v>355</v>
+        <v>359</v>
       </c>
       <c r="D14" t="n">
         <v>12903</v>
       </c>
       <c r="E14" t="n">
-        <v>355</v>
+        <v>359</v>
       </c>
       <c r="F14" t="n">
         <v>12903</v>
       </c>
       <c r="G14" t="n">
-        <v>355</v>
+        <v>359</v>
       </c>
       <c r="H14" t="n">
         <v>12903</v>
       </c>
       <c r="I14" t="n">
-        <v>355</v>
+        <v>359</v>
       </c>
       <c r="J14" t="n">
         <v>12903</v>
@@ -27622,28 +27622,28 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>29303</v>
+        <v>29305</v>
       </c>
       <c r="C15" t="n">
-        <v>662</v>
+        <v>664</v>
       </c>
       <c r="D15" t="n">
         <v>28641</v>
       </c>
       <c r="E15" t="n">
-        <v>662</v>
+        <v>664</v>
       </c>
       <c r="F15" t="n">
         <v>28641</v>
       </c>
       <c r="G15" t="n">
-        <v>662</v>
+        <v>664</v>
       </c>
       <c r="H15" t="n">
         <v>28641</v>
       </c>
       <c r="I15" t="n">
-        <v>662</v>
+        <v>664</v>
       </c>
       <c r="J15" t="n">
         <v>28641</v>
@@ -27656,28 +27656,28 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>20176</v>
+        <v>20177</v>
       </c>
       <c r="C16" t="n">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="D16" t="n">
         <v>19736</v>
       </c>
       <c r="E16" t="n">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="F16" t="n">
         <v>19736</v>
       </c>
       <c r="G16" t="n">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="H16" t="n">
         <v>19736</v>
       </c>
       <c r="I16" t="n">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="J16" t="n">
         <v>19736</v>
@@ -27826,28 +27826,28 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>1048</v>
+        <v>1049</v>
       </c>
       <c r="C21" t="n">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D21" t="n">
         <v>1026</v>
       </c>
       <c r="E21" t="n">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F21" t="n">
         <v>1026</v>
       </c>
       <c r="G21" t="n">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H21" t="n">
         <v>1026</v>
       </c>
       <c r="I21" t="n">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="J21" t="n">
         <v>1026</v>
@@ -27860,28 +27860,28 @@
         </is>
       </c>
       <c r="B22" t="n">
-        <v>1943986</v>
+        <v>1944513</v>
       </c>
       <c r="C22" t="n">
-        <v>40054</v>
+        <v>40581</v>
       </c>
       <c r="D22" t="n">
         <v>1903932</v>
       </c>
       <c r="E22" t="n">
-        <v>40054</v>
+        <v>40581</v>
       </c>
       <c r="F22" t="n">
         <v>1903932</v>
       </c>
       <c r="G22" t="n">
-        <v>40054</v>
+        <v>40581</v>
       </c>
       <c r="H22" t="n">
         <v>1903932</v>
       </c>
       <c r="I22" t="n">
-        <v>40054</v>
+        <v>40581</v>
       </c>
       <c r="J22" t="n">
         <v>1903932</v>
@@ -29283,28 +29283,28 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="C2" t="n">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="D2" t="n">
         <v>5</v>
       </c>
       <c r="E2" t="n">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="F2" t="n">
         <v>5</v>
       </c>
       <c r="G2" t="n">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="H2" t="n">
         <v>5</v>
       </c>
       <c r="I2" t="n">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="J2" t="n">
         <v>5</v>
@@ -29317,28 +29317,28 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>19791.66666666666</v>
+        <v>20127.49999999999</v>
       </c>
       <c r="C3" t="n">
-        <v>-3.637978807091713e-12</v>
+        <v>335.8333333333285</v>
       </c>
       <c r="D3" t="n">
         <v>19791.66666666666</v>
       </c>
       <c r="E3" t="n">
-        <v>-3.637978807091713e-12</v>
+        <v>335.8333333333285</v>
       </c>
       <c r="F3" t="n">
         <v>19791.66666666666</v>
       </c>
       <c r="G3" t="n">
-        <v>-3.637978807091713e-12</v>
+        <v>335.8333333333285</v>
       </c>
       <c r="H3" t="n">
         <v>19791.66666666666</v>
       </c>
       <c r="I3" t="n">
-        <v>-3.637978807091713e-12</v>
+        <v>335.8333333333285</v>
       </c>
       <c r="J3" t="n">
         <v>19791.66666666666</v>
@@ -29351,28 +29351,28 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D4" t="n">
         <v>6</v>
       </c>
       <c r="E4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F4" t="n">
         <v>6</v>
       </c>
       <c r="G4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H4" t="n">
         <v>6</v>
       </c>
       <c r="I4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J4" t="n">
         <v>6</v>
@@ -29419,28 +29419,28 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>3131</v>
+        <v>3214</v>
       </c>
       <c r="C6" t="n">
-        <v>0</v>
+        <v>83</v>
       </c>
       <c r="D6" t="n">
         <v>3131</v>
       </c>
       <c r="E6" t="n">
-        <v>0</v>
+        <v>83</v>
       </c>
       <c r="F6" t="n">
         <v>3131</v>
       </c>
       <c r="G6" t="n">
-        <v>0</v>
+        <v>83</v>
       </c>
       <c r="H6" t="n">
         <v>3131</v>
       </c>
       <c r="I6" t="n">
-        <v>0</v>
+        <v>83</v>
       </c>
       <c r="J6" t="n">
         <v>3131</v>
@@ -29453,28 +29453,28 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>195</v>
+        <v>199</v>
       </c>
       <c r="C7" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D7" t="n">
         <v>195</v>
       </c>
       <c r="E7" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F7" t="n">
         <v>195</v>
       </c>
       <c r="G7" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H7" t="n">
         <v>195</v>
       </c>
       <c r="I7" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="J7" t="n">
         <v>195</v>
@@ -29487,28 +29487,28 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C8" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D8" t="n">
         <v>36</v>
       </c>
       <c r="E8" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F8" t="n">
         <v>36</v>
       </c>
       <c r="G8" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H8" t="n">
         <v>36</v>
       </c>
       <c r="I8" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J8" t="n">
         <v>36</v>
@@ -29521,28 +29521,28 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>282</v>
+        <v>288</v>
       </c>
       <c r="C9" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="D9" t="n">
         <v>282</v>
       </c>
       <c r="E9" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="F9" t="n">
         <v>282</v>
       </c>
       <c r="G9" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="H9" t="n">
         <v>282</v>
       </c>
       <c r="I9" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="J9" t="n">
         <v>282</v>
@@ -29555,28 +29555,28 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="C10" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D10" t="n">
         <v>100</v>
       </c>
       <c r="E10" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F10" t="n">
         <v>100</v>
       </c>
       <c r="G10" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H10" t="n">
         <v>100</v>
       </c>
       <c r="I10" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="J10" t="n">
         <v>100</v>
@@ -29589,28 +29589,28 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>2389</v>
+        <v>2437</v>
       </c>
       <c r="C11" t="n">
-        <v>0</v>
+        <v>48</v>
       </c>
       <c r="D11" t="n">
         <v>2389</v>
       </c>
       <c r="E11" t="n">
-        <v>0</v>
+        <v>48</v>
       </c>
       <c r="F11" t="n">
         <v>2389</v>
       </c>
       <c r="G11" t="n">
-        <v>0</v>
+        <v>48</v>
       </c>
       <c r="H11" t="n">
         <v>2389</v>
       </c>
       <c r="I11" t="n">
-        <v>0</v>
+        <v>48</v>
       </c>
       <c r="J11" t="n">
         <v>2389</v>
@@ -29623,28 +29623,28 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="C12" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D12" t="n">
         <v>151</v>
       </c>
       <c r="E12" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F12" t="n">
         <v>151</v>
       </c>
       <c r="G12" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H12" t="n">
         <v>151</v>
       </c>
       <c r="I12" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="J12" t="n">
         <v>151</v>
@@ -29657,28 +29657,28 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="C13" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D13" t="n">
         <v>182</v>
       </c>
       <c r="E13" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F13" t="n">
         <v>182</v>
       </c>
       <c r="G13" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H13" t="n">
         <v>182</v>
       </c>
       <c r="I13" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J13" t="n">
         <v>182</v>
@@ -29691,28 +29691,28 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>129</v>
+        <v>133</v>
       </c>
       <c r="C14" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D14" t="n">
         <v>129</v>
       </c>
       <c r="E14" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F14" t="n">
         <v>129</v>
       </c>
       <c r="G14" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H14" t="n">
         <v>129</v>
       </c>
       <c r="I14" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="J14" t="n">
         <v>129</v>
@@ -29725,28 +29725,28 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="C15" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D15" t="n">
         <v>94</v>
       </c>
       <c r="E15" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F15" t="n">
         <v>94</v>
       </c>
       <c r="G15" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H15" t="n">
         <v>94</v>
       </c>
       <c r="I15" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="J15" t="n">
         <v>94</v>
@@ -29759,28 +29759,28 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C16" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D16" t="n">
         <v>47</v>
       </c>
       <c r="E16" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F16" t="n">
         <v>47</v>
       </c>
       <c r="G16" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H16" t="n">
         <v>47</v>
       </c>
       <c r="I16" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J16" t="n">
         <v>47</v>
@@ -29861,28 +29861,28 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C19" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D19" t="n">
         <v>2</v>
       </c>
       <c r="E19" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F19" t="n">
         <v>2</v>
       </c>
       <c r="G19" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H19" t="n">
         <v>2</v>
       </c>
       <c r="I19" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J19" t="n">
         <v>2</v>
@@ -29895,28 +29895,28 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>30508</v>
+        <v>31074</v>
       </c>
       <c r="C20" t="n">
-        <v>0</v>
+        <v>566</v>
       </c>
       <c r="D20" t="n">
         <v>30508</v>
       </c>
       <c r="E20" t="n">
-        <v>0</v>
+        <v>566</v>
       </c>
       <c r="F20" t="n">
         <v>30508</v>
       </c>
       <c r="G20" t="n">
-        <v>0</v>
+        <v>566</v>
       </c>
       <c r="H20" t="n">
         <v>30508</v>
       </c>
       <c r="I20" t="n">
-        <v>0</v>
+        <v>566</v>
       </c>
       <c r="J20" t="n">
         <v>30508</v>

</xml_diff>